<commit_message>
Calificaciones Const y Var grupo C
</commit_message>
<xml_diff>
--- a/MONITOR20-2/GC/Constantes y Variabes/revisiónConstyVar.xlsx
+++ b/MONITOR20-2/GC/Constantes y Variabes/revisiónConstyVar.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297EEAB1-39E9-45BD-A38E-0D778066FAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09467545-8002-4ADE-AD9C-EBB466577F44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>NO.</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Vera Campo,Valentina</t>
+  </si>
+  <si>
+    <t>No presenta</t>
   </si>
 </sst>
 </file>
@@ -293,6 +296,15 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -304,15 +316,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,7 +335,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -633,11 +636,11 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="0.140625" customWidth="1"/>
@@ -646,12 +649,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
       <c r="E1" t="s">
         <v>4</v>
       </c>
@@ -669,261 +672,354 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="8">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="8">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="8">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="8">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="8">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="8">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="8">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="8">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="8">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="8">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="8">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="8">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="8">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="8">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="8">
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="8">
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="8">
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="8">
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="8">
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="8">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="8">
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="8">
+      <c r="D23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="8">
+      <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="8">
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="8">
+      <c r="D26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="8">
+      <c r="D27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="5">
         <v>26</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="9">
+      <c r="D28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="6">
         <v>27</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="9">
+      <c r="D29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="6">
         <v>28</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="9">
+      <c r="D30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="6">
         <v>29</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>